<commit_message>
ajustes nos dados do imovel
</commit_message>
<xml_diff>
--- a/reports/imoveis_ativos.xlsx
+++ b/reports/imoveis_ativos.xlsx
@@ -82,7 +82,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -91,8 +91,8 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="31.034831460674155"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="7.9348314606741575"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.88988764044944"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="27.28988764044944"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="25.08988764044944"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.989887640449439"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.98988764044944"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="12.884831460674157"/>
   </cols>
   <sheetData>
@@ -178,29 +178,25 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>Residencial</t>
-        </is>
-      </c>
+      <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>04042-070</t>
+          <t>04516-001</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>Vila Clementino</t>
+          <t>Indianópolis</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>Rua Árabe</t>
+          <t>Avenida Rouxinol</t>
         </is>
       </c>
       <c r="F3" s="3" t="n">
-        <v>59</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="4">
@@ -209,24 +205,28 @@
           <t>Residencial</t>
         </is>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Venda</t>
+        </is>
+      </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>08465-070</t>
+          <t>02925-170</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>Conjunto Habitacional Juscelino Kubitschek</t>
+          <t>Freguesia do Ó</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>Rua Doutor Francisco Bueno Torres</t>
+          <t>Rua Anjos do Mar</t>
         </is>
       </c>
       <c r="F4" s="3" t="n">
-        <v>59</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5">
@@ -235,50 +235,54 @@
           <t>Residencial</t>
         </is>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Venda</t>
+        </is>
+      </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>08260-005</t>
+          <t>02925-170</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>Vila Jacuí</t>
+          <t>Freguesia do Ó</t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>Avenida Jacu-Pêssego</t>
+          <t>Rua Anjos do Mar</t>
         </is>
       </c>
       <c r="F5" s="3" t="n">
-        <v>4710</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Residencial</t>
+          <t>Comercial</t>
         </is>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>05051-00</t>
+          <t>81330-650</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>Vila Romana</t>
+          <t>Fazendinha</t>
         </is>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>Rua Tito</t>
+          <t>Rua Raimundo Teobaldo Costa</t>
         </is>
       </c>
       <c r="F6" s="3" t="n">
-        <v>54</v>
+        <v>2725</v>
       </c>
     </row>
     <row r="7">
@@ -287,136 +291,28 @@
           <t>Residencial</t>
         </is>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Venda</t>
+        </is>
+      </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>05051-00</t>
+          <t>04516-001</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>Vila Romana</t>
+          <t>Indianópolis</t>
         </is>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>Rua Tito</t>
+          <t>Avenida Rouxinol</t>
         </is>
       </c>
       <c r="F7" s="3" t="n">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="inlineStr">
-        <is>
-          <t>Residencial</t>
-        </is>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>05051-00</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>Vila Romana</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="inlineStr">
-        <is>
-          <t>Rua Tito</t>
-        </is>
-      </c>
-      <c r="F8" s="3" t="n">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t>Residencial</t>
-        </is>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="inlineStr">
-        <is>
-          <t>02925-170</t>
-        </is>
-      </c>
-      <c r="D9" s="3" t="inlineStr">
-        <is>
-          <t>Freguesia do Ó</t>
-        </is>
-      </c>
-      <c r="E9" s="3" t="inlineStr">
-        <is>
-          <t>Rua Anjos do Mar</t>
-        </is>
-      </c>
-      <c r="F9" s="3" t="n">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="inlineStr">
-        <is>
-          <t>Residencial</t>
-        </is>
-      </c>
-      <c r="B10" s="3" t="inlineStr">
-        <is>
-          <t>Venda</t>
-        </is>
-      </c>
-      <c r="C10" s="3" t="inlineStr">
-        <is>
-          <t>04042-070</t>
-        </is>
-      </c>
-      <c r="D10" s="3" t="inlineStr">
-        <is>
-          <t>Vila Clementino</t>
-        </is>
-      </c>
-      <c r="E10" s="3" t="inlineStr">
-        <is>
-          <t>Rua Árabe</t>
-        </is>
-      </c>
-      <c r="F10" s="3" t="n">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="inlineStr">
-        <is>
-          <t>Residencial</t>
-        </is>
-      </c>
-      <c r="B11" s="3" t="inlineStr">
-        <is>
-          <t>Venda</t>
-        </is>
-      </c>
-      <c r="C11" s="3" t="inlineStr">
-        <is>
-          <t>08465-120</t>
-        </is>
-      </c>
-      <c r="D11" s="3" t="inlineStr">
-        <is>
-          <t>Conjunto Habitacional Juscelino Kubitschek</t>
-        </is>
-      </c>
-      <c r="E11" s="3" t="inlineStr">
-        <is>
-          <t>Rua Fernandez Palero</t>
-        </is>
-      </c>
-      <c r="F11" s="3" t="n">
-        <v>59</v>
+        <v>1024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>